<commit_message>
[INITIAL COMMIT] Initial Version of System ExtractClientInformation, NavigateToWIDetails, UpdateWorkItems and SHA1 ProcessHash Workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fleusebio\OneDrive - Indra\Documents\UiPath\CalculateClientSecurityHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2359EFA1-A650-45E7-87B2-DEBE55684947}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8686B25-A7C6-4DAA-A392-DCA18BBA510A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t>System1_URL</t>
   </si>
   <si>
-    <t>https://acme-test.uipath.com/</t>
-  </si>
-  <si>
     <t>ACME System URL</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>ACME System Work Items Specific-Page URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com</t>
   </si>
 </sst>
 </file>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -624,43 +624,43 @@
         <v>40</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1669,7 +1669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>